<commit_message>
Users excel sheet with heading row support
</commit_message>
<xml_diff>
--- a/public/imports/providers/users.xlsx
+++ b/public/imports/providers/users.xlsx
@@ -20,7 +20,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course</t>
+  </si>
   <si>
     <t xml:space="preserve">Samson Kyozira</t>
   </si>
@@ -71,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bachelor of Economics and Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sseguya John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificate in Metal Works</t>
   </si>
 </sst>
 </file>
@@ -80,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,6 +122,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,8 +173,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -167,10 +199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -184,42 +216,45 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>256700196655</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>256756999607</v>
+        <v>256700196655</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>256752571043</v>
+        <v>256756999607</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>7</v>
@@ -227,44 +262,72 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>256750947920</v>
+        <v>256752571043</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>256788281012</v>
+        <v>256750947920</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>256788281012</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>256757227400</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>256772554007</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>256757227400</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
+      <c r="E8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>